<commit_message>
Test Cases description files commited
</commit_message>
<xml_diff>
--- a/Test_scenario_cases.xlsx
+++ b/Test_scenario_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Steps_to_get_to_registration_pa" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
   <si>
     <t xml:space="preserve">http://automationpractice.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">General comments:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Tested web page very often returns 508 error. 
+- Difficulties with server access made the test process much longer than it could be.
+- Sample screenshots are commited on repository with project.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Several 508 errors made almost impossible to generate tests report with Allure tool</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Module Name</t>
@@ -85,7 +121,7 @@
     <t xml:space="preserve">Actual Result</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Type</t>
+    <t xml:space="preserve">Test Case Type</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -314,9 +350,6 @@
     <t xml:space="preserve">Empty account creation form displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Case Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_010</t>
   </si>
   <si>
@@ -777,7 +810,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -807,6 +840,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -817,12 +864,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -872,7 +913,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,8 +940,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF7B59"/>
+        <bgColor rgb="FFFF6D6D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF6D6D"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFFF7B59"/>
       </patternFill>
     </fill>
     <fill>
@@ -1018,7 +1065,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1047,8 +1094,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1083,6 +1130,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1095,135 +1146,143 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1231,51 +1290,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1335,17 +1394,17 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FFB85C00"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF6D6D"/>
+      <rgbColor rgb="FFFF7B59"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -1369,7 +1428,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFB85C00"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1392,8 +1451,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1429,36 +1488,47 @@
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="9" t="n">
@@ -1467,53 +1537,65 @@
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="27.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="0"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="14"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
@@ -1535,311 +1617,311 @@
     </row>
     <row r="11" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="15" t="s">
         <v>20</v>
       </c>
+      <c r="H11" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="n">
+      <c r="A12" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="D12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="19" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="G12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="21"/>
       <c r="J12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="n">
+      <c r="A13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="n">
+      <c r="A14" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="26"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="24"/>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="24"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="24"/>
+      <c r="H17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="40.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="n">
+      <c r="A18" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20" t="s">
+      <c r="D18" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="G18" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="24"/>
-    </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="n">
+      <c r="H18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="n">
+      <c r="A20" s="30" t="n">
         <v>9</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="E20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="F20" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="24"/>
+      <c r="G20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="24"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
@@ -1851,9 +1933,10 @@
       <c r="A26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I9"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
@@ -1896,8 +1979,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1918,914 +2001,914 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="33"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="40" t="n">
+      <c r="A5" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="44" t="n">
         <v>44343</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
+      <c r="A6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="A7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="35" t="s">
+      <c r="A8" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="34.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="39" t="s">
+      <c r="A9" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="43"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="33.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="E11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="F11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="44" t="s">
+      <c r="G11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>21</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="42.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="n">
+      <c r="A12" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="46"/>
+      <c r="H12" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="49"/>
       <c r="J12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="n">
+      <c r="A13" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50" t="s">
+      <c r="E13" s="53"/>
+      <c r="F13" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="50"/>
+      <c r="H13" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="53"/>
       <c r="J13" s="0"/>
-      <c r="K13" s="52"/>
+      <c r="K13" s="55"/>
     </row>
     <row r="14" customFormat="false" ht="41.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="n">
+      <c r="A14" s="48" t="n">
         <v>3</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53" t="s">
+      <c r="E14" s="56"/>
+      <c r="F14" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="53"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="52"/>
+      <c r="H14" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="56"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="55"/>
     </row>
     <row r="15" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="n">
+      <c r="A15" s="48" t="n">
         <v>4</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="H15" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
+      <c r="H15" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="45.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="n">
+      <c r="A16" s="48" t="n">
         <v>5</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46" t="s">
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="45"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
+      <c r="H16" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="48"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="n">
+      <c r="A17" s="48" t="n">
         <v>6</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="46" t="s">
+      <c r="G17" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="24"/>
+      <c r="H17" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="48"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="78.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="n">
+      <c r="A18" s="48" t="n">
         <v>7</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H18" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="24"/>
+      <c r="H18" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="48"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="100.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="n">
+      <c r="A19" s="48" t="n">
         <v>8</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="45"/>
-      <c r="J19" s="24"/>
+      <c r="H19" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="48"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="n">
+      <c r="A20" s="48" t="n">
         <v>9</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46" t="s">
+      <c r="E20" s="49"/>
+      <c r="F20" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="45"/>
-      <c r="J20" s="24"/>
+      <c r="H20" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="48"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="45" t="n">
+      <c r="A21" s="48" t="n">
         <v>10</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46" t="s">
+      <c r="E21" s="49"/>
+      <c r="F21" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="H21" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="45"/>
-      <c r="J21" s="24"/>
+      <c r="H21" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="48"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="45" t="n">
+      <c r="A22" s="48" t="n">
         <v>11</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46" t="s">
+      <c r="E22" s="49"/>
+      <c r="F22" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="45"/>
-      <c r="J22" s="24"/>
+      <c r="H22" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="48"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="57.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="45" t="n">
+      <c r="A23" s="48" t="n">
         <v>12</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="45"/>
+      <c r="H23" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="48"/>
     </row>
     <row r="24" customFormat="false" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="45" t="n">
+      <c r="A24" s="48" t="n">
         <v>13</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="45"/>
+      <c r="H24" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="48"/>
     </row>
     <row r="25" customFormat="false" ht="57.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="45" t="n">
+      <c r="A25" s="48" t="n">
         <v>14</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="46" t="s">
+      <c r="G25" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H25" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="45"/>
+      <c r="H25" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" customFormat="false" ht="60.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="45" t="n">
+      <c r="A26" s="48" t="n">
         <v>15</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="F26" s="46" t="s">
+      <c r="F26" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="46" t="s">
+      <c r="G26" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="H26" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="45"/>
+      <c r="H26" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="45" t="n">
+      <c r="A27" s="48" t="n">
         <v>16</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="H27" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="45"/>
+      <c r="H27" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="45" t="n">
+      <c r="A28" s="48" t="n">
         <v>17</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="46" t="s">
+      <c r="G28" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="H28" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" s="45"/>
+      <c r="H28" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="48"/>
     </row>
     <row r="29" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="45" t="n">
+      <c r="A29" s="48" t="n">
         <v>18</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="H29" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="45"/>
+      <c r="H29" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="48"/>
     </row>
     <row r="30" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="45" t="n">
+      <c r="A30" s="48" t="n">
         <v>19</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D30" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="H30" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="45"/>
+      <c r="H30" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="48"/>
     </row>
     <row r="31" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="45" t="n">
+      <c r="A31" s="48" t="n">
         <v>20</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="E31" s="58" t="n">
+      <c r="E31" s="61" t="n">
         <v>22314</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="F31" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="H31" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="45"/>
+      <c r="H31" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45" t="n">
+      <c r="A32" s="48" t="n">
         <v>21</v>
       </c>
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="F32" s="46" t="s">
+      <c r="F32" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G32" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="H32" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="45"/>
+      <c r="H32" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="48"/>
     </row>
     <row r="33" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="45" t="n">
+      <c r="A33" s="48" t="n">
         <v>22</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="E33" s="59" t="n">
+      <c r="E33" s="62" t="n">
         <v>5417543010</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="H33" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="45"/>
+      <c r="H33" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="48"/>
     </row>
     <row r="34" customFormat="false" ht="211.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="45" t="n">
+      <c r="A34" s="48" t="n">
         <v>23</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="60" t="s">
+      <c r="E34" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="G34" s="46" t="s">
+      <c r="G34" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="H34" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="45"/>
+      <c r="H34" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="48"/>
     </row>
     <row r="35" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="45"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="48"/>
     </row>
     <row r="36" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="45"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="45"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="48"/>
     </row>
     <row r="37" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="45"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="45"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="48"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="61"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="62" t="s">
+      <c r="A38" s="64"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="61"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="64"/>
     </row>
     <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="45"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="46" t="s">
+      <c r="A39" s="48"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="45"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="48"/>
     </row>
     <row r="40" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="46" t="s">
+      <c r="A40" s="48"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="45"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="48"/>
     </row>
     <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="46" t="s">
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="45"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="48"/>
     </row>
     <row r="42" customFormat="false" ht="19.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="45"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="46" t="s">
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="45"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="48"/>
     </row>
     <row r="43" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="45"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="46" t="s">
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="45"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="48"/>
     </row>
     <row r="44" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
@@ -2833,111 +2916,111 @@
       <c r="C44" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="45"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="48"/>
     </row>
     <row r="45" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="45"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="48"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="63"/>
+      <c r="A46" s="66"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="66"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="63"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="63"/>
+      <c r="A47" s="66"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="66"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="63"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="63"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="66"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="63"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="63"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="66"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="63"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="63"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="63"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="63"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="66"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="63"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="63"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="66"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="63"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="63"/>
+      <c r="A53" s="66"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
Test Cases descriptions file
</commit_message>
<xml_diff>
--- a/Test_scenario_cases.xlsx
+++ b/Test_scenario_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Steps_to_get_to_registration_pa" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="198">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
@@ -781,22 +781,131 @@
     <t xml:space="preserve">Final page header text is: „MY ACCOUNT”</t>
   </si>
   <si>
-    <t xml:space="preserve">More tests ideas TODO:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify success account creation with all required valid data inputs and in several optional fields.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify success account creation with all required valid data inputs and invalid entry in one optional field.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify possibility to create an account with an email already registered before.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate optional fields of create account form.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify if data given during creation account process corresponds with signed in user profile.</t>
+    <t xml:space="preserve">More tests ideas that could be verified:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify each form field with correct and incorrect input format using boundary values.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verify success account creation with valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">inputs in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">all required and several optional fields.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verify success account creation with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">valid data inputs in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">all required fields and invalid entry in one optional field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verify success account creation with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">valid data inputs in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">all optional fields only.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify an attempt to create an account with an email already registered before.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate optional fields of Create Account form.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verify if data given during creation account process corresponds with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">user profile info while </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Ubuntu"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">signed in .</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if user gets email message with confirmation about created account .</t>
   </si>
   <si>
     <t xml:space="preserve">Etc</t>
@@ -810,7 +919,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -911,6 +1020,11 @@
       <name val="Fira Code"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1065,7 +1179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1328,6 +1442,22 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1451,7 +1581,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1977,10 +2107,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ53"/>
+  <dimension ref="A1:AMJ56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2637,7 +2767,7 @@
       </c>
       <c r="I28" s="48"/>
     </row>
-    <row r="29" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="63.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="48" t="n">
         <v>18</v>
       </c>
@@ -2650,7 +2780,7 @@
       <c r="D29" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="62" t="s">
+      <c r="E29" s="61" t="s">
         <v>159</v>
       </c>
       <c r="F29" s="49" t="s">
@@ -2832,7 +2962,7 @@
       <c r="H37" s="49"/>
       <c r="I37" s="48"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="64"/>
       <c r="B38" s="64"/>
       <c r="C38" s="65" t="s">
@@ -2845,20 +2975,21 @@
       <c r="H38" s="65"/>
       <c r="I38" s="64"/>
     </row>
-    <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="48"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49" t="s">
+    <row r="39" s="68" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="48"/>
-    </row>
-    <row r="40" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="66"/>
+      <c r="AMJ39" s="69"/>
+    </row>
+    <row r="40" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="48"/>
       <c r="B40" s="48"/>
       <c r="C40" s="49" t="s">
@@ -2871,7 +3002,7 @@
       <c r="H40" s="49"/>
       <c r="I40" s="48"/>
     </row>
-    <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="48"/>
       <c r="B41" s="48"/>
       <c r="C41" s="49" t="s">
@@ -2884,7 +3015,7 @@
       <c r="H41" s="49"/>
       <c r="I41" s="48"/>
     </row>
-    <row r="42" customFormat="false" ht="19.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="48"/>
       <c r="B42" s="48"/>
       <c r="C42" s="49" t="s">
@@ -2910,10 +3041,10 @@
       <c r="H43" s="49"/>
       <c r="I43" s="48"/>
     </row>
-    <row r="44" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0" t="s">
+    <row r="44" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49" t="s">
         <v>194</v>
       </c>
       <c r="D44" s="49"/>
@@ -2923,10 +3054,12 @@
       <c r="H44" s="49"/>
       <c r="I44" s="48"/>
     </row>
-    <row r="45" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="48"/>
       <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
+      <c r="C45" s="49" t="s">
+        <v>195</v>
+      </c>
       <c r="D45" s="49"/>
       <c r="E45" s="49"/>
       <c r="F45" s="49"/>
@@ -2934,93 +3067,130 @@
       <c r="H45" s="49"/>
       <c r="I45" s="48"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="66"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="66"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="66"/>
-      <c r="B47" s="66"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="66"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="66"/>
-      <c r="B48" s="66"/>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="66"/>
+    <row r="46" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="48"/>
+    </row>
+    <row r="47" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="33"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="48"/>
+    </row>
+    <row r="48" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="66"/>
-      <c r="B49" s="66"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="67"/>
-      <c r="I49" s="66"/>
+      <c r="A49" s="70"/>
+      <c r="B49" s="70"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="70"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="66"/>
-      <c r="B50" s="66"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="66"/>
+      <c r="A50" s="70"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="71"/>
+      <c r="I50" s="70"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="66"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="66"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="70"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="70"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="66"/>
-      <c r="B52" s="66"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="66"/>
+      <c r="A52" s="70"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
+      <c r="H52" s="71"/>
+      <c r="I52" s="70"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="66"/>
-      <c r="B53" s="66"/>
-      <c r="C53" s="67"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="67"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-      <c r="I53" s="66"/>
+      <c r="A53" s="70"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="70"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="70"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
+      <c r="G54" s="71"/>
+      <c r="H54" s="71"/>
+      <c r="I54" s="70"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="70"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
+      <c r="G55" s="71"/>
+      <c r="H55" s="71"/>
+      <c r="I55" s="70"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="70"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>